<commit_message>
Measures and cognitive load theory
</commit_message>
<xml_diff>
--- a/corpus/corpus.xlsx
+++ b/corpus/corpus.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Desktop/P9/corpus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Desktop/P9/bericht/corpus/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AK$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$AK$147</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="488">
   <si>
     <t>G. Aisch and A. Cox</t>
   </si>
@@ -1476,6 +1476,24 @@
   </si>
   <si>
     <t>A. Tse, M. Duhalde</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/interactive/2018/12/24/climate/how-electricity-generation-changed-in-your-state.html</t>
+  </si>
+  <si>
+    <t>N. Popovich</t>
+  </si>
+  <si>
+    <t>How Does Your State Make Electricity?</t>
+  </si>
+  <si>
+    <t>https://www.forbes.com/sites/energyinnovation/2018/12/03/plunging-prices-mean-building-new-renewable-energy-is-cheaper-than-running-existing-coal/#49ce40231f31</t>
+  </si>
+  <si>
+    <t>Plunging Prices Mean Building New Renewable Energy Is Cheaper Than Running Existing Coal</t>
+  </si>
+  <si>
+    <t>M. Mahajan</t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1845,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1971,6 +1989,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2252,10 +2273,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK147"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:AK149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="125" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2440,6 +2462,9 @@
       <c r="E3" s="1" t="s">
         <v>291</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="L3" s="35">
         <v>1</v>
       </c>
@@ -2493,7 +2518,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" s="38" t="s">
         <v>140</v>
       </c>
@@ -2561,7 +2586,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" s="40" t="s">
         <v>142</v>
       </c>
@@ -2850,7 +2875,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" s="40" t="s">
         <v>156</v>
       </c>
@@ -2916,7 +2941,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" s="38" t="s">
         <v>158</v>
       </c>
@@ -2978,7 +3003,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="40" t="s">
         <v>160</v>
       </c>
@@ -3038,7 +3063,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" s="38" t="s">
         <v>162</v>
       </c>
@@ -3100,7 +3125,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="40" t="s">
         <v>164</v>
       </c>
@@ -3162,7 +3187,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" s="38" t="s">
         <v>166</v>
       </c>
@@ -3301,7 +3326,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" s="38" t="s">
         <v>170</v>
       </c>
@@ -3369,7 +3394,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" s="40" t="s">
         <v>172</v>
       </c>
@@ -3569,7 +3594,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" s="40" t="s">
         <v>181</v>
       </c>
@@ -3636,7 +3661,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" s="38" t="s">
         <v>184</v>
       </c>
@@ -3704,7 +3729,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" s="40" t="s">
         <v>186</v>
       </c>
@@ -3770,7 +3795,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" s="38" t="s">
         <v>189</v>
       </c>
@@ -3836,7 +3861,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" s="40" t="s">
         <v>191</v>
       </c>
@@ -3898,7 +3923,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" s="38" t="s">
         <v>194</v>
       </c>
@@ -3966,7 +3991,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" s="40" t="s">
         <v>196</v>
       </c>
@@ -4095,7 +4120,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" s="40" t="s">
         <v>200</v>
       </c>
@@ -4159,7 +4184,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" s="38" t="s">
         <v>202</v>
       </c>
@@ -4230,7 +4255,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" s="40" t="s">
         <v>204</v>
       </c>
@@ -4299,7 +4324,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" s="40" t="s">
         <v>207</v>
       </c>
@@ -4361,7 +4386,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" s="38" t="s">
         <v>209</v>
       </c>
@@ -4421,7 +4446,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" s="40" t="s">
         <v>211</v>
       </c>
@@ -4483,7 +4508,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" s="38" t="s">
         <v>213</v>
       </c>
@@ -4705,7 +4730,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" s="40" t="s">
         <v>220</v>
       </c>
@@ -4767,7 +4792,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" s="38" t="s">
         <v>225</v>
       </c>
@@ -4829,7 +4854,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" s="40" t="s">
         <v>227</v>
       </c>
@@ -4960,7 +4985,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>233</v>
       </c>
@@ -5026,7 +5051,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" s="6" t="s">
         <v>235</v>
       </c>
@@ -5092,7 +5117,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>237</v>
       </c>
@@ -5160,7 +5185,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6" t="s">
         <v>239</v>
       </c>
@@ -5354,7 +5379,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>248</v>
       </c>
@@ -5487,7 +5512,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" s="6" t="s">
         <v>254</v>
       </c>
@@ -5622,7 +5647,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" s="6" t="s">
         <v>258</v>
       </c>
@@ -5686,7 +5711,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>260</v>
       </c>
@@ -5754,7 +5779,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" s="6" t="s">
         <v>263</v>
       </c>
@@ -5814,7 +5839,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>265</v>
       </c>
@@ -5880,7 +5905,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" s="6" t="s">
         <v>267</v>
       </c>
@@ -6011,7 +6036,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>273</v>
       </c>
@@ -6077,7 +6102,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>275</v>
       </c>
@@ -6285,7 +6310,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>281</v>
       </c>
@@ -6351,7 +6376,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
         <v>283</v>
       </c>
@@ -6419,7 +6444,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="2:37" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>285</v>
       </c>
@@ -6554,7 +6579,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>289</v>
       </c>
@@ -7801,7 +7826,7 @@
       <c r="AJ84" s="41"/>
       <c r="AK84" s="41"/>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>344</v>
       </c>
@@ -7843,7 +7868,7 @@
       <c r="AJ85" s="41"/>
       <c r="AK85" s="41"/>
     </row>
-    <row r="86" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>347</v>
       </c>
@@ -8341,7 +8366,7 @@
       <c r="AJ96" s="41"/>
       <c r="AK96" s="41"/>
     </row>
-    <row r="97" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>472</v>
       </c>
@@ -8373,7 +8398,7 @@
       <c r="AJ97" s="41"/>
       <c r="AK97" s="41"/>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>475</v>
       </c>
@@ -8446,7 +8471,7 @@
       <c r="AJ99" s="41"/>
       <c r="AK99" s="41"/>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>481</v>
       </c>
@@ -8616,7 +8641,7 @@
       <c r="AJ103" s="41"/>
       <c r="AK103" s="41"/>
     </row>
-    <row r="104" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>8</v>
       </c>
@@ -8651,7 +8676,7 @@
       <c r="AJ104" s="41"/>
       <c r="AK104" s="41"/>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>11</v>
       </c>
@@ -8850,7 +8875,7 @@
       <c r="AJ109" s="41"/>
       <c r="AK109" s="41"/>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>30</v>
       </c>
@@ -8885,7 +8910,7 @@
       <c r="AJ110" s="41"/>
       <c r="AK110" s="41"/>
     </row>
-    <row r="111" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>41</v>
       </c>
@@ -8996,7 +9021,7 @@
       <c r="AJ113" s="41"/>
       <c r="AK113" s="41"/>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>50</v>
       </c>
@@ -9031,7 +9056,7 @@
       <c r="AJ114" s="41"/>
       <c r="AK114" s="41"/>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>53</v>
       </c>
@@ -9142,7 +9167,7 @@
       <c r="AJ117" s="41"/>
       <c r="AK117" s="41"/>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>65</v>
       </c>
@@ -9177,7 +9202,7 @@
       <c r="AJ118" s="41"/>
       <c r="AK118" s="41"/>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>71</v>
       </c>
@@ -9221,7 +9246,7 @@
       <c r="AJ119" s="52"/>
       <c r="AK119" s="52"/>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>76</v>
       </c>
@@ -9241,7 +9266,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>82</v>
       </c>
@@ -9261,7 +9286,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>85</v>
       </c>
@@ -9281,7 +9306,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>88</v>
       </c>
@@ -9301,7 +9326,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="124" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>92</v>
       </c>
@@ -9321,7 +9346,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="125" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>98</v>
       </c>
@@ -9373,7 +9398,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="127" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>107</v>
       </c>
@@ -9393,7 +9418,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="128" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>110</v>
       </c>
@@ -9471,7 +9496,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="131" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>118</v>
       </c>
@@ -10443,7 +10468,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="147" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:37" hidden="1" x14ac:dyDescent="0.2">
       <c r="N147" s="57" t="s">
         <v>299</v>
       </c>
@@ -10514,8 +10539,47 @@
         <v>313</v>
       </c>
     </row>
+    <row r="148" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B148" s="66" t="s">
+        <v>484</v>
+      </c>
+      <c r="C148" s="34" t="s">
+        <v>482</v>
+      </c>
+      <c r="D148" s="8">
+        <v>2018</v>
+      </c>
+      <c r="E148" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="149" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B149" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="C149" s="34" t="s">
+        <v>485</v>
+      </c>
+      <c r="D149" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AK143">
+  <autoFilter ref="A1:AK147">
+    <filterColumn colId="11">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState ref="A2:AK147">
       <sortCondition ref="E1:E147"/>
     </sortState>
@@ -10638,6 +10702,8 @@
     <hyperlink ref="C98" r:id="rId115"/>
     <hyperlink ref="C99" r:id="rId116"/>
     <hyperlink ref="C100" r:id="rId117"/>
+    <hyperlink ref="C148" r:id="rId118"/>
+    <hyperlink ref="C149" r:id="rId119" location="49ce40231f31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>